<commit_message>
modifications to Africa Numbers
</commit_message>
<xml_diff>
--- a/Africa_weekly_variant_summary.xlsx
+++ b/Africa_weekly_variant_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,7 +360,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Variant</t>
+          <t>Variant (VOC,VOI,VUM)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -375,270 +375,342 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Date of first case</t>
+          <t>Number of sequences</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total confirmed (sequences at GISAID)</t>
+          <t>Sequences submitted in the last 30 days</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>New cases in last 7 days</t>
+          <t>date of first sequence</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>date of last sequence</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>No of days since last sampling</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alpha</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>VOC-202012/01</t>
+          <t>A.23.1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>B.1.1.7</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2020-08-02</t>
-        </is>
+          <t>A.23.1</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>378</v>
       </c>
       <c r="E2">
-        <v>2064</v>
-      </c>
-      <c r="F2">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2021-08-22</t>
+        </is>
+      </c>
+      <c r="H2">
+        <v>39</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Beta</t>
+          <t>Alpha</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VOC-202012/02</t>
+          <t>VOC-202012/01</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>B.1.351</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2020-05-27</t>
-        </is>
+          <t>B.1.1.7</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>2498</v>
       </c>
       <c r="E3">
-        <v>9640</v>
-      </c>
-      <c r="F3">
-        <v>31</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2020-08-02</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2021-08-27</t>
+        </is>
+      </c>
+      <c r="H3">
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Delta+</t>
+          <t>B.1.1.318</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VOC-21APR-02</t>
+          <t>VUM-2021-06-04</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>B.1.617.2, AY.1, AY.3, AY.4, AY.5, AY.6, AY.7.1, AY.10, AY.11, AY.12, AY.13, AY.14, AY.15, AY.16, AY.17, AY.18, AY.19, AY.20, AY.21, AY.23, AY.24, AY.25</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
+          <t>B.1.1.318</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>465</v>
       </c>
       <c r="E4">
-        <v>9675</v>
-      </c>
-      <c r="F4">
-        <v>728</v>
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2021-01-07</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2021-08-06</t>
+        </is>
+      </c>
+      <c r="H4">
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Eta</t>
+          <t>Beta</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VUI-202102/03</t>
+          <t>VOC-202012/02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>B.1.525</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2020-12-11</t>
-        </is>
+          <t>B.1.351, B.1.351.1, B.1.351.2</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>10022</v>
       </c>
       <c r="E5">
-        <v>820</v>
-      </c>
-      <c r="F5">
-        <v>58</v>
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2020-05-27</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2021-08-27</t>
+        </is>
+      </c>
+      <c r="H5">
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>VUI-16SEP-01</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>C.36.3</t>
+          <t>C.1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C.36.3</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2020-04-26</t>
-        </is>
+          <t>C.1</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>384</v>
       </c>
       <c r="E6">
-        <v>78</v>
-      </c>
-      <c r="F6">
         <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2020-04-12</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2021-06-28</t>
+        </is>
+      </c>
+      <c r="H6">
+        <v>94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>VUI-21FEB-04</t>
+          <t>C.1.2</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VUI-202102/04</t>
+          <t>VUM-2021-09-01</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>B.1.1.318</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2021-01-07</t>
-        </is>
+          <t>C.1.2</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>168</v>
       </c>
       <c r="E7">
-        <v>390</v>
-      </c>
-      <c r="F7">
-        <v>29</v>
+        <v>7</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2021-05-11</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2021-09-09</t>
+        </is>
+      </c>
+      <c r="H7">
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>VUI-21MAY-02</t>
+          <t>C.36.3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>C.1</t>
+          <t>VUM-2021-06-16</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C.1</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2020-04-12</t>
-        </is>
+          <t>C.36.3</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>104</v>
       </c>
       <c r="E8">
-        <v>387</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2020-04-26</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2021-06-16</t>
+        </is>
+      </c>
+      <c r="H8">
+        <v>106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>VUI-21OCT-01</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A.23.1</t>
+          <t>VOC-21APR-02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A.23.1</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2020-10-21</t>
-        </is>
+          <t>B.1.617.2, AY.1, AY.3, AY.4, AY.5, AY.6, AY.7.1, AY.10, AY.11, AY.12, AY.13, AY.14, AY.15, AY.16, AY.17, AY.18, AY.19, AY.20, AY.21, AY.23, AY.24, AY.25</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>12401</v>
       </c>
       <c r="E9">
-        <v>361</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
+        <v>457</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2020-09-16</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2021-09-20</t>
+        </is>
+      </c>
+      <c r="H9">
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>VUI-26JUN-01</t>
+          <t>Eta</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>C.1.2</t>
+          <t>VUM-202102/03</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C.1.2</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2021-05-11</t>
-        </is>
+          <t>B.1.525</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>960</v>
       </c>
       <c r="E10">
-        <v>133</v>
-      </c>
-      <c r="F10">
         <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2020-03-28</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2021-09-16</t>
+        </is>
+      </c>
+      <c r="H10">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of B.1.318 sublineages
</commit_message>
<xml_diff>
--- a/Africa_weekly_variant_summary.xlsx
+++ b/Africa_weekly_variant_summary.xlsx
@@ -479,27 +479,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>B.1.1.318</t>
+          <t>B.1.1.318, AZ.1, AZ.2, AZ.5</t>
         </is>
       </c>
       <c r="D4">
-        <v>465</v>
+        <v>668</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2021-01-07</t>
+          <t>2021-01-06</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2021-08-06</t>
+          <t>2021-08-11</t>
         </is>
       </c>
       <c r="H4">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -661,7 +661,7 @@
         <v>12401</v>
       </c>
       <c r="E9">
-        <v>457</v>
+        <v>422</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Updated voi/voc table) structure and new data upto 14th Oct.
</commit_message>
<xml_diff>
--- a/Africa_weekly_variant_summary.xlsx
+++ b/Africa_weekly_variant_summary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -380,20 +380,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Sequences submitted in the last 30 days</t>
+          <t>Sequences submitted in the last 30 days (data up to 2021-10-14)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>new sequences sampled and submitted in the last 30 days (data up to 2021-10-14)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>date of first sequence</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>date of last sequence</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>No of days since last sampling</t>
         </is>
@@ -402,140 +407,154 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A.23.1</t>
+          <t>Alpha</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>VOC-202012/01</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>A.23.1</t>
+          <t>B.1.1.7</t>
         </is>
       </c>
       <c r="D2">
-        <v>378</v>
+        <v>2564</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2020-10-21</t>
-        </is>
+        <v>399</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2021-08-22</t>
-        </is>
-      </c>
-      <c r="H2">
-        <v>39</v>
+          <t>2020-08-02</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2021-09-30</t>
+        </is>
+      </c>
+      <c r="I2">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Beta</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VOC-202012/01</t>
+          <t>VOC-202012/02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>B.1.1.7</t>
+          <t>B.1.351, B.1.351.1, B.1.351.2</t>
         </is>
       </c>
       <c r="D3">
-        <v>2498</v>
+        <v>10219</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2020-08-02</t>
-        </is>
+        <v>437</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2021-08-27</t>
-        </is>
-      </c>
-      <c r="H3">
-        <v>34</v>
+          <t>2020-05-27</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2021-09-25</t>
+        </is>
+      </c>
+      <c r="I3">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>B.1.1.318</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VUM-2021-06-04</t>
+          <t>VOC-21APR-02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>B.1.1.318, AZ.1, AZ.2, AZ.5</t>
+          <t>B.1.617.2, AY.1, AY.3, AY.4, AY.5, AY.6, AY.7.1, AY.10, AY.11, AY.12, AY.13, AY.14, AY.15, AY.16, AY.17, AY.18, AY.19, AY.20, AY.21, AY.23, AY.24, AY.25</t>
         </is>
       </c>
       <c r="D4">
-        <v>668</v>
+        <v>12722</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2021-01-06</t>
-        </is>
+        <v>3444</v>
+      </c>
+      <c r="F4">
+        <v>52</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2021-08-11</t>
-        </is>
-      </c>
-      <c r="H4">
-        <v>50</v>
+          <t>2020-09-10</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2021-09-20</t>
+        </is>
+      </c>
+      <c r="I4">
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Beta</t>
+          <t>B.1.1.318</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VOC-202012/02</t>
+          <t>VUM-2021-06-04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>B.1.351, B.1.351.1, B.1.351.2</t>
+          <t>B.1.1.318, AZ.1, AZ.2, AZ.5</t>
         </is>
       </c>
       <c r="D5">
-        <v>10022</v>
+        <v>672</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2020-05-27</t>
-        </is>
+        <v>110</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2021-08-27</t>
-        </is>
-      </c>
-      <c r="H5">
-        <v>34</v>
+          <t>2021-01-06</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2021-08-11</t>
+        </is>
+      </c>
+      <c r="I5">
+        <v>66</v>
       </c>
     </row>
     <row r="6">
@@ -552,21 +571,18 @@
       <c r="D6">
         <v>384</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>2020-04-12</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>2021-06-28</t>
         </is>
       </c>
-      <c r="H6">
-        <v>94</v>
+      <c r="I6">
+        <v>110</v>
       </c>
     </row>
     <row r="7">
@@ -586,23 +602,26 @@
         </is>
       </c>
       <c r="D7">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7" t="inlineStr">
+        <v>48</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>2021-05-11</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2021-09-09</t>
-        </is>
-      </c>
-      <c r="H7">
-        <v>21</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2021-09-17</t>
+        </is>
+      </c>
+      <c r="I7">
+        <v>29</v>
       </c>
     </row>
     <row r="8">
@@ -625,92 +644,90 @@
         <v>104</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>2020-04-26</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>2021-06-16</t>
         </is>
       </c>
-      <c r="H8">
-        <v>106</v>
+      <c r="I8">
+        <v>122</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Delta</t>
+          <t>Eta</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>VOC-21APR-02</t>
+          <t>VUM-202102/03</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>B.1.617.2, AY.1, AY.3, AY.4, AY.5, AY.6, AY.7.1, AY.10, AY.11, AY.12, AY.13, AY.14, AY.15, AY.16, AY.17, AY.18, AY.19, AY.20, AY.21, AY.23, AY.24, AY.25</t>
+          <t>B.1.525</t>
         </is>
       </c>
       <c r="D9">
-        <v>12401</v>
+        <v>991</v>
       </c>
       <c r="E9">
-        <v>422</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2020-09-16</t>
-        </is>
+        <v>197</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2021-09-20</t>
-        </is>
-      </c>
-      <c r="H9">
-        <v>10</v>
+          <t>2020-03-28</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2021-09-17</t>
+        </is>
+      </c>
+      <c r="I9">
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Eta</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>VUM-202102/03</t>
+          <t>A.23.1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>B.1.525</t>
+          <t>A.23.1</t>
         </is>
       </c>
       <c r="D10">
-        <v>960</v>
+        <v>388</v>
       </c>
       <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2020-03-28</t>
-        </is>
+        <v>26</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2021-09-16</t>
-        </is>
-      </c>
-      <c r="H10">
-        <v>14</v>
+          <t>2020-10-21</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2021-08-22</t>
+        </is>
+      </c>
+      <c r="I10">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>